<commit_message>
Added more excel files and can read multiple files in one df
</commit_message>
<xml_diff>
--- a/Example Spreadsheets/2017.11.21 1 Oh Heck Score Sheet.xlsx
+++ b/Example Spreadsheets/2017.11.21 1 Oh Heck Score Sheet.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianmcaulay/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="0F4AAACAFC8A3C893094EBFBF6D5D27CF4FD21ED" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171026" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,10 +30,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Enter Bids in green and number of tricks made in blue. Score will be automatically calculated in yellow. </t>
+    <t xml:space="preserve">Enter the number of tricks in the red cell. </t>
   </si>
   <si>
-    <t xml:space="preserve">Enter the number of tricks in the red cell. </t>
+    <t xml:space="preserve">Enter Bids in green and number of tricks made in blue. Score will be automatically calculated in yellow. </t>
   </si>
   <si>
     <t>Brian</t>
@@ -50,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,8 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,20 +267,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -279,6 +280,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -546,97 +550,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="5.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="5" max="5" width="5.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="17.100000000000001" thickBot="1">
+      <c r="B4" s="18">
         <v>12</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="12">
+      <c r="C4" s="18"/>
+      <c r="D4" s="15">
         <f>IF(B4="","",IF(B4&gt;1,B4-1,""))</f>
         <v>11</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15">
         <f>IF(D4="","",IF(D4&gt;1,D4-1,""))</f>
         <v>10</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15">
         <f>IF(F4="","",IF(F4&gt;1,F4-1,""))</f>
         <v>9</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12">
+      <c r="I4" s="15"/>
+      <c r="J4" s="15">
         <f>IF(H4="","",IF(H4&gt;1,H4-1,""))</f>
         <v>8</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12">
+      <c r="K4" s="15"/>
+      <c r="L4" s="15">
         <f>IF(J4="","",IF(J4&gt;1,J4-1,""))</f>
         <v>7</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12">
+      <c r="M4" s="15"/>
+      <c r="N4" s="15">
         <f>IF(L4="","",IF(L4&gt;1,L4-1,""))</f>
         <v>6</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12">
+      <c r="O4" s="15"/>
+      <c r="P4" s="15">
         <f>IF(N4="","",IF(N4&gt;1,N4-1,""))</f>
         <v>5</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12">
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15">
         <f>IF(P4="","",IF(P4&gt;1,P4-1,""))</f>
         <v>4</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12">
+      <c r="S4" s="15"/>
+      <c r="T4" s="15">
         <f>IF(R4="","",IF(R4&gt;1,R4-1,""))</f>
         <v>3</v>
       </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12">
+      <c r="U4" s="15"/>
+      <c r="V4" s="15">
         <f>IF(T4="","",IF(T4&gt;1,T4-1,""))</f>
         <v>2</v>
       </c>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12">
+      <c r="W4" s="15"/>
+      <c r="X4" s="15">
         <f>IF(V4="","",IF(V4&gt;1,V4-1,""))</f>
         <v>1</v>
       </c>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12" t="str">
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15" t="str">
         <f>IF(X4="","",IF(X4&gt;1,X4-1,""))</f>
         <v/>
       </c>
-      <c r="AA4" s="12"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="AA4" s="15"/>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5">
@@ -714,8 +718,8 @@
       <c r="Z5" s="8"/>
       <c r="AA5" s="9"/>
     </row>
-    <row r="6" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:28" ht="17.100000000000001" thickBot="1">
+      <c r="A6" s="16"/>
       <c r="B6" s="4"/>
       <c r="C6" s="10">
         <f>IF(C5 = "", "", IF(B5 = C5, C5 + 10, C5))</f>
@@ -782,8 +786,8 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:28">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="5">
@@ -861,8 +865,8 @@
       <c r="Z7" s="8"/>
       <c r="AA7" s="9"/>
     </row>
-    <row r="8" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:28" ht="17.100000000000001" thickBot="1">
+      <c r="A8" s="17"/>
       <c r="B8" s="4"/>
       <c r="C8" s="10">
         <f>IF(C7 = "", "", IF(B7 = C7, C7 + 10, C7))</f>
@@ -929,8 +933,8 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:28">
+      <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="5">
@@ -1008,8 +1012,8 @@
       <c r="Z9" s="8"/>
       <c r="AA9" s="9"/>
     </row>
-    <row r="10" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:28" ht="17.100000000000001" thickBot="1">
+      <c r="A10" s="17"/>
       <c r="B10" s="4"/>
       <c r="C10" s="10">
         <f>IF(C9 = "", "", IF(B9 = C9, C9 + 10, C9))</f>
@@ -1076,8 +1080,8 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:28">
+      <c r="A11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5">
@@ -1155,8 +1159,8 @@
       <c r="Z11" s="8"/>
       <c r="AA11" s="9"/>
     </row>
-    <row r="12" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:28" ht="17.100000000000001" thickBot="1">
+      <c r="A12" s="17"/>
       <c r="B12" s="4"/>
       <c r="C12" s="10">
         <f>IF(C11 = "", "", IF(B11 = C11, C11 + 10, C11))</f>
@@ -1223,264 +1227,264 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
+    <row r="13" spans="1:28">
+      <c r="A13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="17"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17"/>
-      <c r="AA14" s="17"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="17"/>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="17"/>
-      <c r="AA15" s="17"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="17"/>
-      <c r="X16" s="17"/>
-      <c r="Y16" s="17"/>
-      <c r="Z16" s="17"/>
-      <c r="AA16" s="17"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="17"/>
-      <c r="AA18" s="17"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="17"/>
-      <c r="Y19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="17"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="17"/>
-      <c r="Y20" s="17"/>
-      <c r="Z20" s="17"/>
-      <c r="AA20" s="17"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+    </row>
+    <row r="15" spans="1:28">
+      <c r="A15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+    </row>
+    <row r="22" spans="1:27">
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1489,11 +1493,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="X4:Y4"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -1510,6 +1509,11 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="X4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>